<commit_message>
Versão inicial do app Streamlit
</commit_message>
<xml_diff>
--- a/agentes_pastorais.xlsx
+++ b/agentes_pastorais.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karen\Desktop\Trabalho UNINTER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karen\Desktop\WorkSpace\mapeamento_pastorais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2827974A-817E-45EF-A28D-9386624FB4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188ADB3A-A1C6-49CA-A528-89DCDD986545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{46C2F3EA-499A-4DAE-9C73-3922F1650812}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11295" xr2:uid="{46C2F3EA-499A-4DAE-9C73-3922F1650812}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="127">
   <si>
     <t>ID</t>
   </si>
@@ -270,9 +270,6 @@
   </si>
   <si>
     <t>Dízimo / Liturgia / Batismo</t>
-  </si>
-  <si>
-    <t>“Desde sempre”</t>
   </si>
   <si>
     <t>Rua Paulo Sarmento, nº 45 – Conjunto Amazonino Mendes II</t>
@@ -430,7 +427,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="000"/>
+    <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -498,7 +495,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -840,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028BD6EB-71FB-4364-BC52-B67063C10C96}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,16 +1476,14 @@
         <v>37</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1496,13 +1491,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="E24" s="4">
         <v>14</v>
@@ -1512,12 +1507,12 @@
         <v>10</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1525,7 +1520,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
@@ -1539,7 +1534,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1550,11 +1545,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="4">
         <v>49</v>
@@ -1569,7 +1564,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1577,13 +1572,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="E27" s="4">
         <v>13</v>
@@ -1595,7 +1590,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1606,11 +1601,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" s="4">
         <v>49</v>
@@ -1622,7 +1617,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -1633,10 +1628,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>33</v>
@@ -1660,7 +1655,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
@@ -1672,12 +1667,12 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1685,10 +1680,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>33</v>
@@ -1701,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -1712,13 +1707,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="E32" s="4">
         <v>63</v>
@@ -1730,12 +1725,12 @@
         <v>26</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1743,13 +1738,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>108</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="E33" s="4">
         <v>48</v>
@@ -1759,7 +1754,7 @@
         <v>23</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -1770,13 +1765,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="E34" s="4">
         <v>50</v>
@@ -1786,7 +1781,7 @@
         <v>23</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -1797,10 +1792,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>22</v>
@@ -1815,7 +1810,7 @@
         <v>26</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -1826,10 +1821,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>65</v>
@@ -1842,7 +1837,7 @@
         <v>24</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -1853,13 +1848,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="E37" s="4">
         <v>64</v>
@@ -1871,7 +1866,7 @@
         <v>26</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -1882,7 +1877,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
@@ -1896,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -1907,11 +1902,11 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E39" s="4">
         <v>81</v>
@@ -1928,7 +1923,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>